<commit_message>
Added functionality to the master_problem class. Currently does not work
</commit_message>
<xml_diff>
--- a/master_problem.xlsx
+++ b/master_problem.xlsx
@@ -455,7 +455,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr"/>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Iteration</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Location</t>

</xml_diff>